<commit_message>
Added training data, graphs, and updated Agest Results spreadsheet
</commit_message>
<xml_diff>
--- a/MP4_Reinforcement_Learning/Agents/Training_Data/Agent Results.xlsx
+++ b/MP4_Reinforcement_Learning/Agents/Training_Data/Agent Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szymonkoszarek/Box Sync/UIUC/Semester 6 - SP18/CS-440/MPs/AILIENS/MP4_Reinforcement_Learning/Agents/Training_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAEF3F8-90C0-B642-9A7E-7D66806959F4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFCEAD9-7E9C-224A-9B5B-A05EEB73B201}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="460" windowWidth="18940" windowHeight="14700" xr2:uid="{6CA11537-A84C-E149-B258-65E48BF0FA48}"/>
+    <workbookView xWindow="12220" yWindow="460" windowWidth="13300" windowHeight="14700" xr2:uid="{6CA11537-A84C-E149-B258-65E48BF0FA48}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -130,25 +130,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -156,6 +156,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -183,9 +189,10 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -195,14 +202,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BAD72F6-8F66-F940-B261-729D016EE3B1}" name="Table1" displayName="Table1" ref="A2:G12" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BAD72F6-8F66-F940-B261-729D016EE3B1}" name="Table1" displayName="Table1" ref="A2:G12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A2:G12" xr:uid="{443A770B-E24E-1D45-B699-D43E5E084A43}"/>
   <sortState ref="A3:G12">
     <sortCondition ref="A3:A12"/>
@@ -226,13 +226,13 @@
     <sortCondition ref="C3:C12"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C094D3A5-37B7-164C-A723-6AA2D2A71B84}" name="Learning Rate Constant" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F6DAD6A7-047F-B14D-AFAA-8C7345C61DF6}" name="Discount Factor" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{B4CC92AF-83B9-D445-A53B-1B3AF1677A98}" name="Exploration Threshold" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{43186E2A-D3A4-2C47-A1D0-2851B0299240}" name="Avg Bounces" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{D45D6FAF-2F3F-7548-AEE8-C5DE00198BBC}" name="Max Reward" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{D7C832CB-E96C-A647-8604-FC83E5DA4418}" name="Avg Bounces2" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{C4D1243E-1A8E-8B42-A803-81DDA1B514B9}" name="Max Reward3" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{C094D3A5-37B7-164C-A723-6AA2D2A71B84}" name="Learning Rate Constant" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F6DAD6A7-047F-B14D-AFAA-8C7345C61DF6}" name="Discount Factor" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B4CC92AF-83B9-D445-A53B-1B3AF1677A98}" name="Exploration Threshold" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{43186E2A-D3A4-2C47-A1D0-2851B0299240}" name="Avg Bounces" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{D45D6FAF-2F3F-7548-AEE8-C5DE00198BBC}" name="Max Reward" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D7C832CB-E96C-A647-8604-FC83E5DA4418}" name="Avg Bounces2" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{C4D1243E-1A8E-8B42-A803-81DDA1B514B9}" name="Max Reward3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -538,7 +538,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -555,11 +555,11 @@
       <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -571,10 +571,10 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -594,8 +594,14 @@
       <c r="C3" s="1">
         <v>10</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="1">
+        <v>10.3833</v>
+      </c>
+      <c r="G3" s="1">
+        <v>46.98</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
@@ -607,10 +613,10 @@
       <c r="C4" s="1">
         <v>10</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>10.865</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>49</v>
       </c>
       <c r="F4" s="1">
@@ -630,11 +636,11 @@
       <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="11">
-        <v>11.865</v>
-      </c>
-      <c r="E5" s="8">
-        <v>64</v>
+      <c r="D5" s="8">
+        <v>11.63715</v>
+      </c>
+      <c r="E5" s="6">
+        <v>51.39</v>
       </c>
       <c r="F5" s="1">
         <v>7.1349999999999998</v>
@@ -653,17 +659,17 @@
       <c r="C6" s="1">
         <v>10</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>11.79</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>45</v>
       </c>
       <c r="F6" s="1">
-        <v>10.210000000000001</v>
+        <v>9.8320000000000007</v>
       </c>
       <c r="G6" s="1">
-        <v>49</v>
+        <v>45.44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -676,8 +682,18 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="8">
+        <v>12.884499999999999</v>
+      </c>
+      <c r="E7" s="6">
+        <v>57.52</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.6527999999999992</v>
+      </c>
+      <c r="G7" s="1">
+        <v>38.26</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
@@ -689,10 +705,10 @@
       <c r="C8" s="1">
         <v>20</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>13.39</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>49</v>
       </c>
       <c r="F8" s="1">
@@ -712,10 +728,10 @@
       <c r="C9" s="1">
         <v>10</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>13.77</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>57</v>
       </c>
       <c r="F9" s="1">
@@ -735,10 +751,10 @@
       <c r="C10" s="1">
         <v>10</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>8.9600000000000009</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="6">
         <v>45</v>
       </c>
       <c r="F10" s="1">
@@ -758,17 +774,17 @@
       <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11" s="11">
-        <v>13.105</v>
-      </c>
-      <c r="E11" s="8">
-        <v>50</v>
+      <c r="D11" s="8">
+        <v>13.151999999999999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>58.1</v>
       </c>
       <c r="F11" s="1">
-        <v>8.5500000000000007</v>
+        <v>7.9095500000000003</v>
       </c>
       <c r="G11" s="1">
-        <v>46</v>
+        <v>32.840000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -781,8 +797,18 @@
       <c r="C12" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="8">
+        <v>14.7683</v>
+      </c>
+      <c r="E12" s="6">
+        <v>65.58</v>
+      </c>
+      <c r="F12" s="1">
+        <v>7.7417999999999996</v>
+      </c>
+      <c r="G12" s="1">
+        <v>32.89</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Restored lost agents stats
</commit_message>
<xml_diff>
--- a/MP4_Reinforcement_Learning/Agents/Training_Data/Agent Results.xlsx
+++ b/MP4_Reinforcement_Learning/Agents/Training_Data/Agent Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szymonkoszarek/Box Sync/UIUC/Semester 6 - SP18/CS-440/MPs/AILIENS/MP4_Reinforcement_Learning/Agents/Training_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAEF3F8-90C0-B642-9A7E-7D66806959F4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93807F7D-B751-AE42-B315-3C77ED0D903D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="460" windowWidth="18940" windowHeight="14700" xr2:uid="{6CA11537-A84C-E149-B258-65E48BF0FA48}"/>
+    <workbookView xWindow="12220" yWindow="460" windowWidth="13300" windowHeight="14700" xr2:uid="{6CA11537-A84C-E149-B258-65E48BF0FA48}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -130,25 +130,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -156,6 +156,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -183,9 +189,10 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -195,14 +202,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BAD72F6-8F66-F940-B261-729D016EE3B1}" name="Table1" displayName="Table1" ref="A2:G12" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BAD72F6-8F66-F940-B261-729D016EE3B1}" name="Table1" displayName="Table1" ref="A2:G12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A2:G12" xr:uid="{443A770B-E24E-1D45-B699-D43E5E084A43}"/>
   <sortState ref="A3:G12">
     <sortCondition ref="A3:A12"/>
@@ -226,13 +226,13 @@
     <sortCondition ref="C3:C12"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C094D3A5-37B7-164C-A723-6AA2D2A71B84}" name="Learning Rate Constant" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F6DAD6A7-047F-B14D-AFAA-8C7345C61DF6}" name="Discount Factor" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{B4CC92AF-83B9-D445-A53B-1B3AF1677A98}" name="Exploration Threshold" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{43186E2A-D3A4-2C47-A1D0-2851B0299240}" name="Avg Bounces" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{D45D6FAF-2F3F-7548-AEE8-C5DE00198BBC}" name="Max Reward" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{D7C832CB-E96C-A647-8604-FC83E5DA4418}" name="Avg Bounces2" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{C4D1243E-1A8E-8B42-A803-81DDA1B514B9}" name="Max Reward3" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{C094D3A5-37B7-164C-A723-6AA2D2A71B84}" name="Learning Rate Constant" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F6DAD6A7-047F-B14D-AFAA-8C7345C61DF6}" name="Discount Factor" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B4CC92AF-83B9-D445-A53B-1B3AF1677A98}" name="Exploration Threshold" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{43186E2A-D3A4-2C47-A1D0-2851B0299240}" name="Avg Bounces" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{D45D6FAF-2F3F-7548-AEE8-C5DE00198BBC}" name="Max Reward" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D7C832CB-E96C-A647-8604-FC83E5DA4418}" name="Avg Bounces2" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{C4D1243E-1A8E-8B42-A803-81DDA1B514B9}" name="Max Reward3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7319D9-30CB-034A-9139-C735ED370B07}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -555,11 +555,11 @@
       <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -571,10 +571,10 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -594,8 +594,18 @@
       <c r="C3" s="1">
         <v>10</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="8">
+        <v>12.0397</v>
+      </c>
+      <c r="E3" s="6">
+        <v>51.8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10.3833</v>
+      </c>
+      <c r="G3" s="1">
+        <v>46.98</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
@@ -607,10 +617,10 @@
       <c r="C4" s="1">
         <v>10</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>10.865</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>49</v>
       </c>
       <c r="F4" s="1">
@@ -630,17 +640,17 @@
       <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="11">
-        <v>11.865</v>
-      </c>
-      <c r="E5" s="8">
-        <v>64</v>
+      <c r="D5" s="8">
+        <v>11.63715</v>
+      </c>
+      <c r="E5" s="6">
+        <v>51.39</v>
       </c>
       <c r="F5" s="1">
-        <v>7.1349999999999998</v>
+        <v>7.2368499999999996</v>
       </c>
       <c r="G5" s="1">
-        <v>27</v>
+        <v>32.71</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -653,17 +663,17 @@
       <c r="C6" s="1">
         <v>10</v>
       </c>
-      <c r="D6" s="11">
-        <v>11.79</v>
-      </c>
-      <c r="E6" s="8">
-        <v>45</v>
+      <c r="D6" s="8">
+        <v>12.0967</v>
+      </c>
+      <c r="E6" s="6">
+        <v>54.95</v>
       </c>
       <c r="F6" s="1">
-        <v>10.210000000000001</v>
+        <v>9.8320000000000007</v>
       </c>
       <c r="G6" s="1">
-        <v>49</v>
+        <v>45.44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -676,8 +686,18 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="8">
+        <v>12.884499999999999</v>
+      </c>
+      <c r="E7" s="6">
+        <v>57.52</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.6527999999999992</v>
+      </c>
+      <c r="G7" s="1">
+        <v>38.26</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
@@ -689,17 +709,17 @@
       <c r="C8" s="1">
         <v>20</v>
       </c>
-      <c r="D8" s="11">
-        <v>13.39</v>
-      </c>
-      <c r="E8" s="8">
-        <v>49</v>
+      <c r="D8" s="8">
+        <v>13.095800000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>55.27</v>
       </c>
       <c r="F8" s="1">
-        <v>10.404999999999999</v>
+        <v>10.513450000000001</v>
       </c>
       <c r="G8" s="1">
-        <v>65</v>
+        <v>47.43</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -712,10 +732,10 @@
       <c r="C9" s="1">
         <v>10</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>13.77</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>57</v>
       </c>
       <c r="F9" s="1">
@@ -735,10 +755,10 @@
       <c r="C10" s="1">
         <v>10</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>8.9600000000000009</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="6">
         <v>45</v>
       </c>
       <c r="F10" s="1">
@@ -758,17 +778,17 @@
       <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11" s="11">
-        <v>13.105</v>
-      </c>
-      <c r="E11" s="8">
-        <v>50</v>
+      <c r="D11" s="8">
+        <v>13.151999999999999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>58.1</v>
       </c>
       <c r="F11" s="1">
-        <v>8.5500000000000007</v>
+        <v>7.9095500000000003</v>
       </c>
       <c r="G11" s="1">
-        <v>46</v>
+        <v>32.840000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -781,8 +801,18 @@
       <c r="C12" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="8">
+        <v>14.7683</v>
+      </c>
+      <c r="E12" s="6">
+        <v>65.58</v>
+      </c>
+      <c r="F12" s="1">
+        <v>7.7417999999999996</v>
+      </c>
+      <c r="G12" s="1">
+        <v>32.89</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated Agent Results spreadsheet
</commit_message>
<xml_diff>
--- a/MP4_Reinforcement_Learning/Agents/Training_Data/Agent Results.xlsx
+++ b/MP4_Reinforcement_Learning/Agents/Training_Data/Agent Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szymonkoszarek/Box Sync/UIUC/Semester 6 - SP18/CS-440/MPs/AILIENS/MP4_Reinforcement_Learning/Agents/Training_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93807F7D-B751-AE42-B315-3C77ED0D903D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EBAB94-80DD-0549-8523-9D3C2CA11CF8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12220" yWindow="460" windowWidth="13300" windowHeight="14700" xr2:uid="{6CA11537-A84C-E149-B258-65E48BF0FA48}"/>
+    <workbookView xWindow="-80" yWindow="460" windowWidth="13300" windowHeight="14700" xr2:uid="{6CA11537-A84C-E149-B258-65E48BF0FA48}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +149,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -222,8 +225,8 @@
   <autoFilter ref="A2:G12" xr:uid="{443A770B-E24E-1D45-B699-D43E5E084A43}"/>
   <sortState ref="A3:G12">
     <sortCondition ref="A3:A12"/>
+    <sortCondition ref="C3:C12"/>
     <sortCondition ref="B3:B12"/>
-    <sortCondition ref="C3:C12"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C094D3A5-37B7-164C-A723-6AA2D2A71B84}" name="Learning Rate Constant" dataDxfId="6"/>
@@ -537,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7319D9-30CB-034A-9139-C735ED370B07}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -618,16 +621,16 @@
         <v>10</v>
       </c>
       <c r="D4" s="8">
-        <v>10.865</v>
+        <v>11.8756</v>
       </c>
       <c r="E4" s="6">
-        <v>49</v>
+        <v>53.31</v>
       </c>
       <c r="F4" s="1">
-        <v>10.875</v>
+        <v>10.507099999999999</v>
       </c>
       <c r="G4" s="1">
-        <v>35</v>
+        <v>45.62</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -704,22 +707,22 @@
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C8" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8">
-        <v>13.095800000000001</v>
+        <v>13.529299999999999</v>
       </c>
       <c r="E8" s="6">
-        <v>55.27</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10.513450000000001</v>
-      </c>
-      <c r="G8" s="1">
-        <v>47.43</v>
+        <v>58.84</v>
+      </c>
+      <c r="F8" s="12">
+        <v>9.3723500000000008</v>
+      </c>
+      <c r="G8" s="12">
+        <v>39.200000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -727,22 +730,22 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
       </c>
       <c r="D9" s="8">
-        <v>13.77</v>
+        <v>8.7409999999999997</v>
       </c>
       <c r="E9" s="6">
-        <v>57</v>
-      </c>
-      <c r="F9" s="1">
-        <v>9.6</v>
-      </c>
-      <c r="G9" s="1">
-        <v>40</v>
+        <v>36.92</v>
+      </c>
+      <c r="F9" s="8">
+        <v>8.3331499999999998</v>
+      </c>
+      <c r="G9" s="6">
+        <v>33.840000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -750,22 +753,22 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C10" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D10" s="8">
-        <v>8.9600000000000009</v>
+        <v>13.095800000000001</v>
       </c>
       <c r="E10" s="6">
-        <v>45</v>
+        <v>55.27</v>
       </c>
       <c r="F10" s="1">
-        <v>8.0549999999999997</v>
+        <v>10.513450000000001</v>
       </c>
       <c r="G10" s="1">
-        <v>47</v>
+        <v>47.43</v>
       </c>
     </row>
     <row r="11" spans="1:7">

</xml_diff>